<commit_message>
upgraded to version 1.12.0.0
</commit_message>
<xml_diff>
--- a/examples/basetables/xlsx/vpc.xlsx
+++ b/examples/basetables/xlsx/vpc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/tabular-terraform/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/tabular-terraform/examples/basetables/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B680D44-715A-EF4F-9431-B1EB33F4AE9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4206C4-528A-0746-99F4-F246D5DD2631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="3060" windowWidth="19160" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7980" yWindow="3060" windowWidth="19160" windowHeight="12180" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpcs" sheetId="56" r:id="rId1"/>
@@ -22,6 +22,11 @@
     <sheet name="images" sheetId="52" r:id="rId7"/>
     <sheet name="floatingips" sheetId="54" r:id="rId8"/>
     <sheet name="publicgateways" sheetId="55" r:id="rId9"/>
+    <sheet name="instancegroups" sheetId="58" r:id="rId10"/>
+    <sheet name="instancemanagers" sheetId="59" r:id="rId11"/>
+    <sheet name="instancepolicies" sheetId="60" r:id="rId12"/>
+    <sheet name="instancetemplates" sheetId="61" r:id="rId13"/>
+    <sheet name="flowlogs" sheetId="62" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="76">
   <si>
     <t>public_gateway</t>
   </si>
@@ -180,6 +185,93 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>*instance_template</t>
+  </si>
+  <si>
+    <t>*instance_count</t>
+  </si>
+  <si>
+    <t>*subnets</t>
+  </si>
+  <si>
+    <t>application_port</t>
+  </si>
+  <si>
+    <t>load_balancer</t>
+  </si>
+  <si>
+    <t>load_balancer_pool</t>
+  </si>
+  <si>
+    <t>*instance_group</t>
+  </si>
+  <si>
+    <t>*max_membership_count</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>enable_manager</t>
+  </si>
+  <si>
+    <t>manager_type</t>
+  </si>
+  <si>
+    <t>aggregation_window</t>
+  </si>
+  <si>
+    <t>cooldown</t>
+  </si>
+  <si>
+    <t>min_membership_count</t>
+  </si>
+  <si>
+    <t>*policy_type</t>
+  </si>
+  <si>
+    <t>*instance_group_manager</t>
+  </si>
+  <si>
+    <t>metrc_type</t>
+  </si>
+  <si>
+    <t>metric_value</t>
+  </si>
+  <si>
+    <t>primary_network_interface.primary_ipv4_address</t>
+  </si>
+  <si>
+    <t>network_interfaces.primary_ipv4_address</t>
+  </si>
+  <si>
+    <t>boot_volumn.size</t>
+  </si>
+  <si>
+    <t>boot_volume.profile</t>
+  </si>
+  <si>
+    <t>boot_volume.delete_volume_on_instance_delete</t>
+  </si>
+  <si>
+    <t>volume_attachments.name</t>
+  </si>
+  <si>
+    <t>volume_attachments.volume</t>
+  </si>
+  <si>
+    <t>volume_attachments.delete_volume_on_instance_delete</t>
+  </si>
+  <si>
+    <t>*target</t>
+  </si>
+  <si>
+    <t>*storage_bucket</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -303,16 +395,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="123">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="203">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -359,126 +442,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -612,6 +575,421 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -757,186 +1135,301 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9570D1AD-4F2D-D14C-8C67-0A975A90B837}" name="Table3" displayName="Table3" ref="A1:H4" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9570D1AD-4F2D-D14C-8C67-0A975A90B837}" name="Table3" displayName="Table3" ref="A1:H4" totalsRowShown="0" headerRowDxfId="202" dataDxfId="201">
   <autoFilter ref="A1:H4" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{340E4F10-C339-F64A-B4A0-6BA91FA595D8}" name="*file" dataDxfId="120"/>
-    <tableColumn id="1" xr3:uid="{292111BE-F2D3-0E46-9DFF-5BB162CDEBCD}" name="*resource" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{59F12491-5EFE-F14F-B220-749D24D90C3B}" name="*name" dataDxfId="118"/>
-    <tableColumn id="6" xr3:uid="{C8DC1E69-1D37-9E4B-B372-E3771052041B}" name="address_prefix_management" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{85521486-0C28-4E42-A5DD-305E9413CE33}" name="classic_access" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{B1695B9B-C8E2-6B40-822B-13E24CFC2F72}" name="resource_group" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{7270DC4E-CCCE-4547-B9C9-693DFDABB9B7}" name="tags" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{79C76CE0-ABAF-144C-995C-4803DD7D5317}" name="comments" dataDxfId="113"/>
+    <tableColumn id="7" xr3:uid="{340E4F10-C339-F64A-B4A0-6BA91FA595D8}" name="*file" dataDxfId="200"/>
+    <tableColumn id="1" xr3:uid="{292111BE-F2D3-0E46-9DFF-5BB162CDEBCD}" name="*resource" dataDxfId="199"/>
+    <tableColumn id="2" xr3:uid="{59F12491-5EFE-F14F-B220-749D24D90C3B}" name="*name" dataDxfId="198"/>
+    <tableColumn id="6" xr3:uid="{C8DC1E69-1D37-9E4B-B372-E3771052041B}" name="address_prefix_management" dataDxfId="197"/>
+    <tableColumn id="5" xr3:uid="{85521486-0C28-4E42-A5DD-305E9413CE33}" name="classic_access" dataDxfId="196"/>
+    <tableColumn id="3" xr3:uid="{B1695B9B-C8E2-6B40-822B-13E24CFC2F72}" name="resource_group" dataDxfId="195"/>
+    <tableColumn id="4" xr3:uid="{7270DC4E-CCCE-4547-B9C9-693DFDABB9B7}" name="tags" dataDxfId="194"/>
+    <tableColumn id="8" xr3:uid="{79C76CE0-ABAF-144C-995C-4803DD7D5317}" name="comments" dataDxfId="193"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE6D2FD5-EB0A-8E4D-8F9D-447078EE58E0}" name="Table32362" displayName="Table32362" ref="A1:N5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+  <autoFilter ref="A1:N5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="14">
+    <tableColumn id="7" xr3:uid="{A3DEC567-28DD-D444-8C55-48BD2C22DBFB}" name="*file" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{22EB785F-7F8D-2A48-8DAE-E656F83642F1}" name="*resource" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{CC689669-ECA3-C341-A175-9A9EBBCB0163}" name="*name" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{AF511FFE-2094-854A-ADF4-FEAC3BAF7901}" name="*instance_template" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{B1DF2EB5-9A17-5240-B39C-2919D27D9046}" name="*instance_count" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{27BF0027-864A-2E4D-9CA5-0D294F8AE7F8}" name="*subnets" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{AD41D0B5-D757-4E4E-8C7F-B7C05B07B2FB}" name="application_port" dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{ACB33795-12FA-9847-B2BE-E61FF03A7990}" name="load_balancer" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{EF26D84D-2C63-D342-9800-21CB1670BCD2}" name="load_balancer_pool" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{A7E97BBF-5E4D-EA4D-82A2-5509FE2ED286}" name="resource_group" dataDxfId="71"/>
+    <tableColumn id="12" xr3:uid="{D59D4B6F-304B-154B-9427-A03EBA180548}" name="timeout.create" dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{E76FB5A9-577E-3B44-B7DA-565C65F3C1FB}" name="timeout.update" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{69E5EB29-D63E-834A-8A2C-32020A3A2E46}" name="timeout.delete" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{B74C7B3C-2DBD-134F-B119-4925F9D4440C}" name="comments" dataDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8C1365E7-926F-8A4F-9B93-93ABCE4902A0}" name="Table323625" displayName="Table323625" ref="A1:K5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="A1:K5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="11">
+    <tableColumn id="7" xr3:uid="{2C7FBC1F-3C33-4742-A5CE-C1CDA242B38A}" name="*file" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{31906970-3826-CB47-A30E-AB46E5A9E36A}" name="*resource" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{08C11E92-71C9-D74A-AF26-F431D42A26A2}" name="name" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{79D012E3-035F-A341-AC9A-323E0CACBF3B}" name="*instance_group" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{B9064698-EAFB-DE44-BDA4-19F9C9016A22}" name="enable_manager" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{08070EF4-4CEC-8343-BB1E-AF87B1FCD2C0}" name="manager_type" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{99861ADF-7866-2240-A512-09894CB6EEBD}" name="aggregation_window" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{36740D1D-70F4-E344-B71C-A8FBB0BE57B3}" name="cooldown" dataDxfId="54"/>
+    <tableColumn id="15" xr3:uid="{E4C7C17D-BFC1-104A-9247-537522E11462}" name="*max_membership_count" dataDxfId="52"/>
+    <tableColumn id="16" xr3:uid="{7905F2C5-7B98-DC4C-9332-D0F9A4D9D22C}" name="min_membership_count" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{4A8F1306-30CE-BC43-A4B1-F3660C171A85}" name="comments" dataDxfId="53"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B05A9B5E-94AF-3E47-A263-ABAC6BE5815A}" name="Table3236259" displayName="Table3236259" ref="A1:I5" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+  <autoFilter ref="A1:I5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="9">
+    <tableColumn id="7" xr3:uid="{078CA018-6E21-4142-9E49-556AC1004A4D}" name="*file" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{02470F09-766F-B147-9722-CA30A7F5485A}" name="*resource" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{8FA831FD-D30B-0144-8FA5-D029A82F587D}" name="name" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{B4605EFD-F758-1C45-BB22-6E6B1AA8FCE4}" name="*policy_type" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{6AA0E361-6BE8-384B-B237-C1F506694FB2}" name="*instance_group" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{C1C1C1B0-D08D-0F40-8C08-E6377A8F208F}" name="*instance_group_manager" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{2D462E1B-C256-494D-A927-1A7B3ECC4FE6}" name="metrc_type" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{1957482D-EEA4-1F46-AC07-1E2D9DD491CB}" name="metric_value" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{E4117FD4-F44A-6A44-8276-08BF7FDCBE36}" name="comments" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{6A850D06-89D5-5147-9FC1-7C57889F83A4}" name="Table714" displayName="Table714" ref="A1:AA5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:AA5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="27">
+    <tableColumn id="11" xr3:uid="{ABD8360A-CA45-1841-AC25-A7A4F000DCE3}" name="*file" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{DA1D24F0-C40C-974A-947C-C7F1C1400D57}" name="*resource" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{9EA7704F-8643-AA47-A770-E26A648BC400}" name="*name" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{013E55CE-C1AC-0147-9672-ED17FAE5D20B}" name="*vpc" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{96A36CCF-4E4B-A34E-BC3E-B7B3E5240662}" name="*zone" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{8553F152-3CE6-684F-9FCD-7BD79D7EE9D5}" name="*profile" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{DF67DC36-0A14-4449-BE87-A639B8D04BFE}" name="*image" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{08394C5F-12B7-CF41-A513-72E24DDB5B87}" name="boot_volume.name" dataDxfId="30"/>
+    <tableColumn id="22" xr3:uid="{16108B96-DFB1-234A-875A-95F64FAC388C}" name="boot_volume.encryption" dataDxfId="29"/>
+    <tableColumn id="27" xr3:uid="{D9835BE2-5621-2E40-BB7A-3F3255031D00}" name="boot_volumn.size" dataDxfId="15"/>
+    <tableColumn id="28" xr3:uid="{9990D938-3A33-9949-BF83-76D350C7A279}" name="boot_volume.profile" dataDxfId="14"/>
+    <tableColumn id="29" xr3:uid="{804E472F-FD11-BD44-AE26-43984D26CA2E}" name="boot_volume.delete_volume_on_instance_delete" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{490625BA-29F8-C34D-9AA1-2E9C8CBD7587}" name="*keys" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{7B3294C8-68A8-014E-8E86-DA6EC8A9E908}" name="primary_network_interface.name" dataDxfId="27"/>
+    <tableColumn id="21" xr3:uid="{3BFF7C11-0231-854E-B307-5D892BC94035}" name="*primary_network_interface.subnet" dataDxfId="26"/>
+    <tableColumn id="20" xr3:uid="{9790B056-7DC5-3849-B12C-ED0001A5730C}" name="primary_network_interface.security_groups" dataDxfId="25"/>
+    <tableColumn id="25" xr3:uid="{A8315C04-FD3E-504E-A306-24BDDACAA2B6}" name="primary_network_interface.primary_ipv4_address" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{2184C022-C261-F24B-8434-3EEFD88593BA}" name="network_interfaces.name" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{A40B24DE-EF7C-3E46-92FC-7A911DAB37B6}" name="network_interfaces.subnet" dataDxfId="23"/>
+    <tableColumn id="23" xr3:uid="{ED200ECD-DF3A-4842-AF32-2214FD174A2E}" name="network_interfaces.security_groups" dataDxfId="22"/>
+    <tableColumn id="26" xr3:uid="{841931F6-C7D8-F040-9C7D-4A5FFACD93FA}" name="network_interfaces.primary_ipv4_address" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{D1188084-5FC4-7448-B43B-281226F6DA78}" name="volume_attachments.name" dataDxfId="21"/>
+    <tableColumn id="30" xr3:uid="{A82F68A2-9208-C24D-8E2A-50C2D713C90D}" name="volume_attachments.volume" dataDxfId="12"/>
+    <tableColumn id="31" xr3:uid="{1BFA27AC-D95B-7645-B18B-95047504C938}" name="volume_attachments.delete_volume_on_instance_delete" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{27D9D24E-86A1-3A4B-9ACE-DBDB11C7E748}" name="user_data" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{97D29F11-41DF-4D4F-AB7C-578B6C43A348}" name="resource_group" dataDxfId="19"/>
+    <tableColumn id="24" xr3:uid="{B775D107-CE75-DE41-BBBB-EDE63D257826}" name="comments" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F5FD735C-0AC0-C249-8593-4AB77C4361C0}" name="Table3231015" displayName="Table3231015" ref="A1:I8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I8" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="9">
+    <tableColumn id="9" xr3:uid="{20940755-9956-434D-BB5B-0A87046922EB}" name="*file" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{C1895D5E-15F6-C94F-9A8C-B14B0F349DF6}" name="*resource" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{7D0EA6FD-C627-3348-9991-F184C84B9F7D}" name="*name" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{2E062B49-A7B1-CB46-993D-BE94BE132826}" name="*target" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{642A67C8-BB5E-F249-8053-551099048C36}" name="*storage_bucket" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{79FD8B89-DB86-B14B-9047-932EB5B8CA7C}" name="active" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{7E054372-B452-3242-A7C5-8DCA80CDB3FD}" name="resource_group" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{DF4979E3-F869-C04F-9D2D-0A486F93FC3A}" name="tags" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{49BA36C7-5636-CD49-97A7-61E281774763}" name="comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{80D0EAB6-24C7-A740-BC9D-6186BC8E6FB5}" name="Table313" displayName="Table313" ref="A1:G5" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{80D0EAB6-24C7-A740-BC9D-6186BC8E6FB5}" name="Table313" displayName="Table313" ref="A1:G5" totalsRowShown="0" headerRowDxfId="192" dataDxfId="191">
   <autoFilter ref="A1:G5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{CA8AE98B-6B50-E24F-B2BD-282CD5516C27}" name="*file" dataDxfId="110"/>
-    <tableColumn id="1" xr3:uid="{3BCC355B-620B-6847-AC9E-522468082D6D}" name="*resource" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{1A7EE2EF-ECAA-C24E-BE7F-BDC7E7C66612}" name="*name" dataDxfId="108"/>
-    <tableColumn id="6" xr3:uid="{7280C63B-6C9E-4B48-92B0-A3F1288C1832}" name="*vpc" dataDxfId="107"/>
-    <tableColumn id="5" xr3:uid="{0C1D8608-7A3A-B048-96C1-D354FEEA65A3}" name="*zone" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{A0A75B9A-7A60-5C49-AC20-4546ED8ECB0D}" name="cidr" dataDxfId="105"/>
-    <tableColumn id="7" xr3:uid="{8758895A-D42B-674D-BDF6-A66939975CE1}" name="comments" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{CA8AE98B-6B50-E24F-B2BD-282CD5516C27}" name="*file" dataDxfId="190"/>
+    <tableColumn id="1" xr3:uid="{3BCC355B-620B-6847-AC9E-522468082D6D}" name="*resource" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{1A7EE2EF-ECAA-C24E-BE7F-BDC7E7C66612}" name="*name" dataDxfId="188"/>
+    <tableColumn id="6" xr3:uid="{7280C63B-6C9E-4B48-92B0-A3F1288C1832}" name="*vpc" dataDxfId="187"/>
+    <tableColumn id="5" xr3:uid="{0C1D8608-7A3A-B048-96C1-D354FEEA65A3}" name="*zone" dataDxfId="186"/>
+    <tableColumn id="4" xr3:uid="{A0A75B9A-7A60-5C49-AC20-4546ED8ECB0D}" name="cidr" dataDxfId="185"/>
+    <tableColumn id="7" xr3:uid="{8758895A-D42B-674D-BDF6-A66939975CE1}" name="comments" dataDxfId="184"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:H5" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7E4E482-6BB9-E248-AF8D-C5304BC1A44F}" name="Table3236" displayName="Table3236" ref="A1:H5" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182">
   <autoFilter ref="A1:H5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{CE9B09DC-223D-5948-AC6B-A4581B87B9FF}" name="*file" dataDxfId="101"/>
-    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*resource" dataDxfId="100"/>
-    <tableColumn id="6" xr3:uid="{EE4AA5A4-75BE-FF4E-8F15-36A9E95772C8}" name="*name" dataDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="95"/>
-    <tableColumn id="8" xr3:uid="{E7227433-2B78-9D4D-8881-D527D5A672B7}" name="comments" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{CE9B09DC-223D-5948-AC6B-A4581B87B9FF}" name="*file" dataDxfId="181"/>
+    <tableColumn id="1" xr3:uid="{60C065E1-55B2-104C-9BD3-648FFAC30A51}" name="*resource" dataDxfId="180"/>
+    <tableColumn id="6" xr3:uid="{EE4AA5A4-75BE-FF4E-8F15-36A9E95772C8}" name="*name" dataDxfId="179"/>
+    <tableColumn id="3" xr3:uid="{8BD05EA0-AFD7-AF41-B934-9ECEE2438312}" name="*vpc" dataDxfId="178"/>
+    <tableColumn id="2" xr3:uid="{92355D65-8FB2-FA47-80DC-D34EF9FEADBD}" name="*zone" dataDxfId="177"/>
+    <tableColumn id="4" xr3:uid="{EF21D846-0B2C-9441-B0FD-2EA28736C729}" name="*destination" dataDxfId="176"/>
+    <tableColumn id="5" xr3:uid="{7D2B7989-C527-9D46-A034-89A1FB4BA0D5}" name="*next_hop" dataDxfId="175"/>
+    <tableColumn id="8" xr3:uid="{E7227433-2B78-9D4D-8881-D527D5A672B7}" name="comments" dataDxfId="174"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:O14" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:O14" totalsRowShown="0" headerRowDxfId="173" dataDxfId="172">
   <autoFilter ref="A1:O14" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*file" dataDxfId="91"/>
-    <tableColumn id="20" xr3:uid="{5943CD7A-B5EC-7B40-8BA3-EBD8220428FF}" name="*resource" dataDxfId="90"/>
-    <tableColumn id="13" xr3:uid="{D3929CC1-816E-924A-B3D9-F8BE28A4FD4C}" name="*name" dataDxfId="89"/>
-    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="86"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="83"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{9F7D1843-FE18-EE45-A0D8-E33F82A21A7E}" name="resource_group" dataDxfId="81"/>
-    <tableColumn id="15" xr3:uid="{7567182C-2521-7148-9E1E-B075E05FD1EF}" name="timeout.create" dataDxfId="80"/>
-    <tableColumn id="14" xr3:uid="{4ACD08CD-3C38-7244-A429-7A0C64B01515}" name="timeout.update" dataDxfId="79"/>
-    <tableColumn id="16" xr3:uid="{604C7CD3-60C9-9B43-9759-6426B139DA7C}" name="timeout.delete" dataDxfId="78"/>
-    <tableColumn id="8" xr3:uid="{82B01E0D-ECB0-024D-B579-25B381FC228D}" name="comments" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*file" dataDxfId="171"/>
+    <tableColumn id="20" xr3:uid="{5943CD7A-B5EC-7B40-8BA3-EBD8220428FF}" name="*resource" dataDxfId="170"/>
+    <tableColumn id="13" xr3:uid="{D3929CC1-816E-924A-B3D9-F8BE28A4FD4C}" name="*name" dataDxfId="169"/>
+    <tableColumn id="11" xr3:uid="{9C2673D8-AB9A-9645-A3ED-D9B779022434}" name="*vpc" dataDxfId="168"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="167"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="166"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="165"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="164"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="163"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="162"/>
+    <tableColumn id="12" xr3:uid="{9F7D1843-FE18-EE45-A0D8-E33F82A21A7E}" name="resource_group" dataDxfId="161"/>
+    <tableColumn id="15" xr3:uid="{7567182C-2521-7148-9E1E-B075E05FD1EF}" name="timeout.create" dataDxfId="160"/>
+    <tableColumn id="14" xr3:uid="{4ACD08CD-3C38-7244-A429-7A0C64B01515}" name="timeout.update" dataDxfId="159"/>
+    <tableColumn id="16" xr3:uid="{604C7CD3-60C9-9B43-9759-6426B139DA7C}" name="timeout.delete" dataDxfId="158"/>
+    <tableColumn id="8" xr3:uid="{82B01E0D-ECB0-024D-B579-25B381FC228D}" name="comments" dataDxfId="157"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:X11" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:X11" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155">
   <autoFilter ref="A1:X11" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="24">
-    <tableColumn id="11" xr3:uid="{C312D547-C899-B54A-8C78-2627C59BE698}" name="*file" dataDxfId="74"/>
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*resource" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{B05647B5-4075-584D-BFA2-184B7558EF5E}" name="*name" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="68"/>
-    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume.name" dataDxfId="67"/>
-    <tableColumn id="22" xr3:uid="{EE5AAA60-CB22-C74A-9CC2-D51DD5B0DD65}" name="boot_volume.encryption" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="primary_network_interface.name" dataDxfId="64"/>
-    <tableColumn id="21" xr3:uid="{DDD37876-0117-6140-842E-18A729C330C8}" name="*primary_network_interface.subnet" dataDxfId="63"/>
-    <tableColumn id="20" xr3:uid="{EC1E0AEE-B8DD-2145-B373-A9AEFFCF12E6}" name="primary_network_interface.security_groups" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces.name" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{21E0F340-105F-0540-B4FF-9EF83CAC0917}" name="network_interfaces.subnet" dataDxfId="60"/>
-    <tableColumn id="23" xr3:uid="{F3FE0F95-9B4D-5C46-AA1B-68E7C904AEEF}" name="network_interfaces.security_groups" dataDxfId="59"/>
-    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="58"/>
-    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="57"/>
-    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{E502A166-3100-FF4A-9402-397D4F4E4E1A}" name="tags" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="timeout_create" dataDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{35D34496-719B-A04D-99AA-CD60179A1A6E}" name="timeout_delete" dataDxfId="53"/>
-    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="count" dataDxfId="52"/>
-    <tableColumn id="24" xr3:uid="{E4D23545-B894-EB46-8FB9-A2EF7A1F55DC}" name="comments" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{C312D547-C899-B54A-8C78-2627C59BE698}" name="*file" dataDxfId="154"/>
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*resource" dataDxfId="153"/>
+    <tableColumn id="8" xr3:uid="{B05647B5-4075-584D-BFA2-184B7558EF5E}" name="*name" dataDxfId="152"/>
+    <tableColumn id="7" xr3:uid="{AECA3B2B-972B-2947-B76F-3FE48277F64A}" name="*vpc" dataDxfId="151"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="150"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="149"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="*image" dataDxfId="148"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume.name" dataDxfId="147"/>
+    <tableColumn id="22" xr3:uid="{EE5AAA60-CB22-C74A-9CC2-D51DD5B0DD65}" name="boot_volume.encryption" dataDxfId="146"/>
+    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="145"/>
+    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="primary_network_interface.name" dataDxfId="144"/>
+    <tableColumn id="21" xr3:uid="{DDD37876-0117-6140-842E-18A729C330C8}" name="*primary_network_interface.subnet" dataDxfId="143"/>
+    <tableColumn id="20" xr3:uid="{EC1E0AEE-B8DD-2145-B373-A9AEFFCF12E6}" name="primary_network_interface.security_groups" dataDxfId="142"/>
+    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces.name" dataDxfId="141"/>
+    <tableColumn id="16" xr3:uid="{21E0F340-105F-0540-B4FF-9EF83CAC0917}" name="network_interfaces.subnet" dataDxfId="140"/>
+    <tableColumn id="23" xr3:uid="{F3FE0F95-9B4D-5C46-AA1B-68E7C904AEEF}" name="network_interfaces.security_groups" dataDxfId="139"/>
+    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="138"/>
+    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="137"/>
+    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="136"/>
+    <tableColumn id="5" xr3:uid="{E502A166-3100-FF4A-9402-397D4F4E4E1A}" name="tags" dataDxfId="135"/>
+    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="timeout_create" dataDxfId="134"/>
+    <tableColumn id="15" xr3:uid="{35D34496-719B-A04D-99AA-CD60179A1A6E}" name="timeout_delete" dataDxfId="133"/>
+    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="count" dataDxfId="132"/>
+    <tableColumn id="24" xr3:uid="{E4D23545-B894-EB46-8FB9-A2EF7A1F55DC}" name="comments" dataDxfId="131"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:N5" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:N5" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
   <autoFilter ref="A1:N5" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
   <tableColumns count="14">
-    <tableColumn id="15" xr3:uid="{9E45B3FE-088C-1043-8CD4-79D757E3B113}" name="*file" dataDxfId="48"/>
-    <tableColumn id="14" xr3:uid="{ADA7B05E-2042-0842-B4FA-B8F9422C32EC}" name="*resource" dataDxfId="47"/>
-    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*profile" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*zone" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="39"/>
-    <tableColumn id="13" xr3:uid="{6B77DCCF-F340-0A42-B34C-B1E50E6E3A9E}" name="tags" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="timeout.create" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="timeout.delete" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{9D59BAAA-3EFD-6942-B905-A5F0EA231122}" name="comments" dataDxfId="35"/>
+    <tableColumn id="15" xr3:uid="{9E45B3FE-088C-1043-8CD4-79D757E3B113}" name="*file" dataDxfId="128"/>
+    <tableColumn id="14" xr3:uid="{ADA7B05E-2042-0842-B4FA-B8F9422C32EC}" name="*resource" dataDxfId="127"/>
+    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*profile" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*zone" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="119"/>
+    <tableColumn id="13" xr3:uid="{6B77DCCF-F340-0A42-B34C-B1E50E6E3A9E}" name="tags" dataDxfId="118"/>
+    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="timeout.create" dataDxfId="117"/>
+    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="timeout.delete" dataDxfId="116"/>
+    <tableColumn id="11" xr3:uid="{9D59BAAA-3EFD-6942-B905-A5F0EA231122}" name="comments" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CC6AE3F-9734-ED45-8903-103E4A3651C5}" name="Table323" displayName="Table323" ref="A1:G5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CC6AE3F-9734-ED45-8903-103E4A3651C5}" name="Table323" displayName="Table323" ref="A1:G5" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
   <autoFilter ref="A1:G5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="7">
-    <tableColumn id="6" xr3:uid="{C8FF2734-BE1B-0842-8813-8FC327A9774A}" name="*resource" dataDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{9D2269D2-DAC7-7A44-AA65-217A6B5A9326}" name="*name" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{AA9DBEBB-EC6B-E848-9DA7-CEA5574D32E3}" name="*href" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{4531D242-4648-604D-A4F0-6C45B93511A5}" name="*operating_system" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{820303A7-0B6A-BA48-B2C6-0BCED3884DAB}" name="resource_group" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{6B88A27A-C37D-D440-A63A-59083B5F8D69}" name="tags" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{985DA3EA-C986-E04C-808D-664748575A40}" name="comments" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C8FF2734-BE1B-0842-8813-8FC327A9774A}" name="*resource" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{9D2269D2-DAC7-7A44-AA65-217A6B5A9326}" name="*name" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{AA9DBEBB-EC6B-E848-9DA7-CEA5574D32E3}" name="*href" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{4531D242-4648-604D-A4F0-6C45B93511A5}" name="*operating_system" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{820303A7-0B6A-BA48-B2C6-0BCED3884DAB}" name="resource_group" dataDxfId="108"/>
+    <tableColumn id="5" xr3:uid="{6B88A27A-C37D-D440-A63A-59083B5F8D69}" name="tags" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{985DA3EA-C986-E04C-808D-664748575A40}" name="comments" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6552C07F-EB8B-624C-B923-480C01A6D118}" name="Table32310" displayName="Table32310" ref="A1:J8" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6552C07F-EB8B-624C-B923-480C01A6D118}" name="Table32310" displayName="Table32310" ref="A1:J8" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
   <autoFilter ref="A1:J8" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{F2E90068-5C88-AB45-95BB-D7ED929152A5}" name="*file" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{4A0384A9-C294-4546-AAA8-D2CD531C4DD5}" name="*resource" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{92E92614-F08C-C24C-BC25-EFF06E49A7B0}" name="*name" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{A4B81C57-BCB8-1145-A862-A8022AC95A72}" name="target" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{2FAC087F-4C6B-A54B-AC75-F25799387B85}" name="zone" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{E0D1E75B-B4E8-D34A-A3B6-40995A6B8667}" name="resource_group" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{EF2FB7C8-85F5-D14F-B25F-863F24D248CF}" name="timeout.create" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{CB52DB2E-8120-844C-878A-453EB7AF6172}" name="timeout.delete" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{CFBD67C6-4C5E-D143-9FC9-4B9B0A3F0F65}" name="count" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{0BA18536-D878-914B-BAAD-43ECB39D0955}" name="comments" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{F2E90068-5C88-AB45-95BB-D7ED929152A5}" name="*file" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{4A0384A9-C294-4546-AAA8-D2CD531C4DD5}" name="*resource" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{92E92614-F08C-C24C-BC25-EFF06E49A7B0}" name="*name" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{A4B81C57-BCB8-1145-A862-A8022AC95A72}" name="target" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{2FAC087F-4C6B-A54B-AC75-F25799387B85}" name="zone" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{E0D1E75B-B4E8-D34A-A3B6-40995A6B8667}" name="resource_group" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{EF2FB7C8-85F5-D14F-B25F-863F24D248CF}" name="timeout.create" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{CB52DB2E-8120-844C-878A-453EB7AF6172}" name="timeout.delete" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{CFBD67C6-4C5E-D143-9FC9-4B9B0A3F0F65}" name="count" dataDxfId="95"/>
+    <tableColumn id="10" xr3:uid="{0BA18536-D878-914B-BAAD-43ECB39D0955}" name="comments" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{84124973-0DD2-E14C-AE4F-009FA40F3C90}" name="Table3231011" displayName="Table3231011" ref="A1:L5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{84124973-0DD2-E14C-AE4F-009FA40F3C90}" name="Table3231011" displayName="Table3231011" ref="A1:L5" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A1:L5" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="12">
-    <tableColumn id="9" xr3:uid="{BBE2BEDB-BA14-AF4C-8145-72293C7E410B}" name="*file" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{56966C65-6E92-2B49-9AD5-52AF7A1437DE}" name="*resource" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{C12BE473-955B-BF41-90F6-8A401D694011}" name="*name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{554340C2-5543-584F-B46A-49C958EA5A44}" name="*vpc" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{0A93D9DD-D272-A74A-9699-52C56DBF2F0B}" name="*zone" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{3AE82495-6BD6-564F-8CF5-EE6F402D714E}" name="floating_ip.id" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{0F341D72-00E6-0E46-A5E4-3EF40F663948}" name="floating_ip.address" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{A73C8507-7B71-B54C-B6A9-8EB6B72CC2BD}" name="resource_controller_url" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{14EA033B-8397-1E4C-BC95-D8C4A8353921}" name="resource_group" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{96188887-86BE-214B-88C8-BBAE7AB7037F}" name="timeout.create" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A106A0EE-A8AF-2348-A534-07EB8E396F98}" name="timeout.delete" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{18943A5F-A2F6-5F4E-9358-2351A368DBFA}" name="comments" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{BBE2BEDB-BA14-AF4C-8145-72293C7E410B}" name="*file" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{56966C65-6E92-2B49-9AD5-52AF7A1437DE}" name="*resource" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{C12BE473-955B-BF41-90F6-8A401D694011}" name="*name" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{554340C2-5543-584F-B46A-49C958EA5A44}" name="*vpc" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{0A93D9DD-D272-A74A-9699-52C56DBF2F0B}" name="*zone" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{3AE82495-6BD6-564F-8CF5-EE6F402D714E}" name="floating_ip.id" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{0F341D72-00E6-0E46-A5E4-3EF40F663948}" name="floating_ip.address" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{A73C8507-7B71-B54C-B6A9-8EB6B72CC2BD}" name="resource_controller_url" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{14EA033B-8397-1E4C-BC95-D8C4A8353921}" name="resource_group" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{96188887-86BE-214B-88C8-BBAE7AB7037F}" name="timeout.create" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{A106A0EE-A8AF-2348-A534-07EB8E396F98}" name="timeout.delete" dataDxfId="81"/>
+    <tableColumn id="12" xr3:uid="{18943A5F-A2F6-5F4E-9358-2351A368DBFA}" name="comments" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1207,7 +1700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13FDFB22-8BE6-E54E-B5DD-237ED87A155B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1275,6 +1768,752 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2163FCBB-4D78-0243-AA81-C266A40310E5}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6E5A69-9265-BE47-A6E6-89879A14540B}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB50CC90-DE28-F74A-8272-406875EAD6CC}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B845252-6D0C-A54D-8987-CFF44B975940}">
+  <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="43" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB92B2B-E0B9-EE4E-B5B6-649AE0D080E5}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1463,7 +2702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E633D9-8336-4776-A01F-1859C551A2C4}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="J1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1774,7 +3013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:X9"/>
     </sheetView>
   </sheetViews>

</xml_diff>